<commit_message>
Adding SCC $1367 option
</commit_message>
<xml_diff>
--- a/data/1_assumptions/default_assumptions_toggles_vMAIN.xlsx
+++ b/data/1_assumptions/default_assumptions_toggles_vMAIN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethuo\Dropbox (MIT)\Regulation\code_files\1_assumptions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethuo\Documents\GitHub\mvpf-climate\data\1_assumptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111FBB6D-5E61-42E2-8C4A-50A0F3D0B31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75AD5C8-BA7C-41C7-86B1-98D767C2B5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-4290" windowWidth="28995" windowHeight="15675" tabRatio="906" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="906" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SELECTIONS" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="117" sheetId="3" r:id="rId3"/>
     <sheet name="193" sheetId="6" r:id="rId4"/>
     <sheet name="337" sheetId="7" r:id="rId5"/>
-    <sheet name="AP3Model_unweighted" sheetId="4" r:id="rId6"/>
-    <sheet name="AP3Model_weighted" sheetId="8" r:id="rId7"/>
+    <sheet name="1367" sheetId="10" r:id="rId6"/>
+    <sheet name="AP3Model_unweighted" sheetId="4" r:id="rId7"/>
+    <sheet name="AP3Model_weighted" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>USShareFutureSSC</t>
   </si>
@@ -109,6 +110,15 @@
   </si>
   <si>
     <t>md_CO</t>
+  </si>
+  <si>
+    <t>sc_old_CO2_193</t>
+  </si>
+  <si>
+    <t>sc_old_CH4_193</t>
+  </si>
+  <si>
+    <t>sc_old_N2O_193</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1076,8 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3902,7 +3912,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5575,12 +5585,12 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -6731,6 +6741,2842 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66B87C3-24A9-4543-9C95-59D4AD257255}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:H97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1985</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C35" si="0">(1 - (((F2-F3)/F3) * -1))*C3</f>
+        <v>419.37631622931195</v>
+      </c>
+      <c r="D2">
+        <f>G2 * (C2/F2)</f>
+        <v>7.0829015544041464E-13</v>
+      </c>
+      <c r="E2">
+        <f>H2*(C2/F2)</f>
+        <v>61387.165050978103</v>
+      </c>
+      <c r="F2">
+        <v>59.2096774193542</v>
+      </c>
+      <c r="G2">
+        <v>1E-13</v>
+      </c>
+      <c r="H2">
+        <v>8666.9516129032709</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1986</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>446.27991810128538</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="1">G3 * (C3/F3)</f>
+        <v>7.0829015544041464E-13</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="2">H3*(C3/F3)</f>
+        <v>70496.473316060874</v>
+      </c>
+      <c r="F3">
+        <v>63.008064516128798</v>
+      </c>
+      <c r="G3">
+        <v>1E-13</v>
+      </c>
+      <c r="H3">
+        <v>9953.0499999998137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1987</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>473.18351997325885</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041454E-13</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>79605.781581146919</v>
+      </c>
+      <c r="F4">
+        <v>66.806451612903402</v>
+      </c>
+      <c r="G4">
+        <v>1E-13</v>
+      </c>
+      <c r="H4">
+        <v>11239.148387096822</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1988</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>500.08712184522591</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041454E-13</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>88715.08984622969</v>
+      </c>
+      <c r="F5">
+        <v>70.604838709677097</v>
+      </c>
+      <c r="G5">
+        <v>1E-13</v>
+      </c>
+      <c r="H5">
+        <v>12525.246774193365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1989</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>526.99072371719944</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041464E-13</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>97824.398111315779</v>
+      </c>
+      <c r="F6">
+        <v>74.403225806451701</v>
+      </c>
+      <c r="G6">
+        <v>1E-13</v>
+      </c>
+      <c r="H6">
+        <v>13811.345161290374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1990</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>553.89432558916644</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041454E-13</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>106933.70637639852</v>
+      </c>
+      <c r="F7">
+        <v>78.201612903225396</v>
+      </c>
+      <c r="G7">
+        <v>1E-13</v>
+      </c>
+      <c r="H7">
+        <v>15097.443548386917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1991</v>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>580.79792746113992</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041454E-13</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>116043.01464148459</v>
+      </c>
+      <c r="F8">
+        <v>82</v>
+      </c>
+      <c r="G8">
+        <v>1E-13</v>
+      </c>
+      <c r="H8">
+        <v>16383.541935483925</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1992</v>
+      </c>
+      <c r="B9">
+        <v>2020</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>607.70152933310692</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041444E-13</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>125152.32290656735</v>
+      </c>
+      <c r="F9">
+        <v>85.798387096773695</v>
+      </c>
+      <c r="G9">
+        <v>1E-13</v>
+      </c>
+      <c r="H9">
+        <v>17669.640322580468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1993</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>634.6051312050804</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041444E-13</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>134261.6311716534</v>
+      </c>
+      <c r="F10">
+        <v>89.596774193548299</v>
+      </c>
+      <c r="G10">
+        <v>1E-13</v>
+      </c>
+      <c r="H10">
+        <v>18955.738709677476</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1994</v>
+      </c>
+      <c r="B11">
+        <v>2020</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>661.50873307704751</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041454E-13</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>143370.9394367362</v>
+      </c>
+      <c r="F11">
+        <v>93.395161290321994</v>
+      </c>
+      <c r="G11">
+        <v>1E-13</v>
+      </c>
+      <c r="H11">
+        <v>20241.837096774019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1995</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>688.41233494902099</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041454E-13</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>152480.24770182226</v>
+      </c>
+      <c r="F12">
+        <v>97.193548387096598</v>
+      </c>
+      <c r="G12">
+        <v>1E-13</v>
+      </c>
+      <c r="H12">
+        <v>21527.935483871028</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1996</v>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>715.31593682098799</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041444E-13</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>161589.555966905</v>
+      </c>
+      <c r="F13">
+        <v>100.99193548387029</v>
+      </c>
+      <c r="G13">
+        <v>1E-13</v>
+      </c>
+      <c r="H13">
+        <v>22814.033870967571</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1997</v>
+      </c>
+      <c r="B14">
+        <v>2020</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>742.21953869296146</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041444E-13</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>170698.86423199109</v>
+      </c>
+      <c r="F14">
+        <v>104.7903225806449</v>
+      </c>
+      <c r="G14">
+        <v>1E-13</v>
+      </c>
+      <c r="H14">
+        <v>24100.132258064579</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1998</v>
+      </c>
+      <c r="B15">
+        <v>2020</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>769.12314056493494</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041444E-13</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>179808.17249707383</v>
+      </c>
+      <c r="F15">
+        <v>108.5887096774195</v>
+      </c>
+      <c r="G15">
+        <v>1E-13</v>
+      </c>
+      <c r="H15">
+        <v>25386.230645161122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1999</v>
+      </c>
+      <c r="B16">
+        <v>2020</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>796.02674243690194</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041434E-13</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>188917.48076215989</v>
+      </c>
+      <c r="F16">
+        <v>112.3870967741932</v>
+      </c>
+      <c r="G16">
+        <v>1E-13</v>
+      </c>
+      <c r="H16">
+        <v>26672.329032258131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>2020</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>822.93034430887542</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041434E-13</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>198026.78902724266</v>
+      </c>
+      <c r="F17">
+        <v>116.1854838709678</v>
+      </c>
+      <c r="G17">
+        <v>1E-13</v>
+      </c>
+      <c r="H17">
+        <v>27958.427419354673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2001</v>
+      </c>
+      <c r="B18">
+        <v>2020</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>849.83394618084242</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>7.0829015544041434E-13</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>207136.09729232872</v>
+      </c>
+      <c r="F18">
+        <v>119.9838709677415</v>
+      </c>
+      <c r="G18">
+        <v>1E-13</v>
+      </c>
+      <c r="H18">
+        <v>29244.525806451682</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2002</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>876.7375480528159</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>166.44247451099642</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>216245.40555741146</v>
+      </c>
+      <c r="F19">
+        <v>123.7822580645161</v>
+      </c>
+      <c r="G19">
+        <v>23.499193548370386</v>
+      </c>
+      <c r="H19">
+        <v>30530.624193548225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2003</v>
+      </c>
+      <c r="B20">
+        <v>2020</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>903.64114992478301</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>778.75360187181616</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>225354.71382249755</v>
+      </c>
+      <c r="F20">
+        <v>127.58064516128979</v>
+      </c>
+      <c r="G20">
+        <v>109.94838709675241</v>
+      </c>
+      <c r="H20">
+        <v>31816.722580645233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2004</v>
+      </c>
+      <c r="B21">
+        <v>2020</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>930.54475179675649</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>1391.064729232636</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>234464.02208758029</v>
+      </c>
+      <c r="F21">
+        <v>131.3790322580644</v>
+      </c>
+      <c r="G21">
+        <v>196.39758064513444</v>
+      </c>
+      <c r="H21">
+        <v>33102.820967741776</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2005</v>
+      </c>
+      <c r="B22">
+        <v>2020</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>957.4483536687236</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2003.3758565936621</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>243573.33035266641</v>
+      </c>
+      <c r="F22">
+        <v>135.17741935483809</v>
+      </c>
+      <c r="G22">
+        <v>282.84677419354557</v>
+      </c>
+      <c r="H22">
+        <v>34388.919354838785</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2006</v>
+      </c>
+      <c r="B23">
+        <v>2020</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>984.35195554069708</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2615.686983954482</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>252682.63861774915</v>
+      </c>
+      <c r="F23">
+        <v>138.9758064516127</v>
+      </c>
+      <c r="G23">
+        <v>369.2959677419276</v>
+      </c>
+      <c r="H23">
+        <v>35675.017741935328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2007</v>
+      </c>
+      <c r="B24">
+        <v>2020</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1011.2555574126706</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>3227.9981113153017</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>261791.94688283524</v>
+      </c>
+      <c r="F24">
+        <v>142.7741935483873</v>
+      </c>
+      <c r="G24">
+        <v>455.74516129030962</v>
+      </c>
+      <c r="H24">
+        <v>36961.116129032336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2008</v>
+      </c>
+      <c r="B25">
+        <v>2020</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>1038.1591592846376</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>3840.3092386761209</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>270901.25514791795</v>
+      </c>
+      <c r="F25">
+        <v>146.572580645161</v>
+      </c>
+      <c r="G25">
+        <v>542.19435483869165</v>
+      </c>
+      <c r="H25">
+        <v>38247.214516128879</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2009</v>
+      </c>
+      <c r="B26">
+        <v>2020</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>1065.062761156611</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>4452.620366036941</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>280010.56341300404</v>
+      </c>
+      <c r="F26">
+        <v>150.3709677419356</v>
+      </c>
+      <c r="G26">
+        <v>628.64354838707368</v>
+      </c>
+      <c r="H26">
+        <v>39533.312903225888</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2010</v>
+      </c>
+      <c r="B27">
+        <v>2020</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>1091.9663630285781</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>5064.9314933977612</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>289119.87167808681</v>
+      </c>
+      <c r="F27">
+        <v>154.1693548387093</v>
+      </c>
+      <c r="G27">
+        <v>715.09274193545571</v>
+      </c>
+      <c r="H27">
+        <v>40819.41129032243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2011</v>
+      </c>
+      <c r="B28">
+        <v>2020</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>1118.8699649005516</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>5677.2426207587869</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>298229.1799431729</v>
+      </c>
+      <c r="F28">
+        <v>157.9677419354839</v>
+      </c>
+      <c r="G28">
+        <v>801.54193548386684</v>
+      </c>
+      <c r="H28">
+        <v>42105.509677419439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2012</v>
+      </c>
+      <c r="B29">
+        <v>2020</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1145.7735667725187</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>6289.553748119607</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>307338.48820825567</v>
+      </c>
+      <c r="F29">
+        <v>161.7661290322576</v>
+      </c>
+      <c r="G29">
+        <v>887.99112903224886</v>
+      </c>
+      <c r="H29">
+        <v>43391.608064515982</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2013</v>
+      </c>
+      <c r="B30">
+        <v>2020</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1172.6771686444922</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>6901.8648754804262</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>316447.7964733417</v>
+      </c>
+      <c r="F30">
+        <v>165.5645161290322</v>
+      </c>
+      <c r="G30">
+        <v>974.44032258063089</v>
+      </c>
+      <c r="H30">
+        <v>44677.70645161299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31">
+        <v>2020</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1199.5807705164593</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>7514.1760028412464</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>325557.10473842447</v>
+      </c>
+      <c r="F31">
+        <v>169.36290322580589</v>
+      </c>
+      <c r="G31">
+        <v>1060.8895161290129</v>
+      </c>
+      <c r="H31">
+        <v>45963.804838709533</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2015</v>
+      </c>
+      <c r="B32">
+        <v>2020</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>1226.4843723884328</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>8126.4871302020665</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>334666.41300351056</v>
+      </c>
+      <c r="F32">
+        <v>173.1612903225805</v>
+      </c>
+      <c r="G32">
+        <v>1147.3387096773949</v>
+      </c>
+      <c r="H32">
+        <v>47249.903225806542</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2016</v>
+      </c>
+      <c r="B33">
+        <v>2020</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1253.3879742603999</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>8738.7982575628866</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>343775.72126859339</v>
+      </c>
+      <c r="F33">
+        <v>176.95967741935419</v>
+      </c>
+      <c r="G33">
+        <v>1233.787903225777</v>
+      </c>
+      <c r="H33">
+        <v>48536.001612903085</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2017</v>
+      </c>
+      <c r="B34">
+        <v>2020</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1280.2915761323734</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>9351.1093849239132</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>352885.02953367942</v>
+      </c>
+      <c r="F34">
+        <v>180.7580645161288</v>
+      </c>
+      <c r="G34">
+        <v>1320.2370967741881</v>
+      </c>
+      <c r="H34">
+        <v>49822.100000000093</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2018</v>
+      </c>
+      <c r="B35">
+        <v>2020</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1307.1951780043469</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>9963.4205122847325</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>361994.33779876219</v>
+      </c>
+      <c r="F35">
+        <v>184.5564516129034</v>
+      </c>
+      <c r="G35">
+        <v>1406.6862903225701</v>
+      </c>
+      <c r="H35">
+        <v>51108.198387096636</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2019</v>
+      </c>
+      <c r="B36">
+        <v>2020</v>
+      </c>
+      <c r="C36">
+        <f>(1 - (((F36-F37)/F37) * -1))*C37</f>
+        <v>1334.098779876314</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>10575.731639645554</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>371103.64606384828</v>
+      </c>
+      <c r="F36">
+        <v>188.3548387096771</v>
+      </c>
+      <c r="G36">
+        <v>1493.1354838709522</v>
+      </c>
+      <c r="H36">
+        <v>52394.296774193645</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>11672.621761658032</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>383461.20725388604</v>
+      </c>
+      <c r="F37" s="2">
+        <v>193</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1648</v>
+      </c>
+      <c r="H37" s="2">
+        <v>54139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2021</v>
+      </c>
+      <c r="B38">
+        <v>2020</v>
+      </c>
+      <c r="C38">
+        <f>(1 + ((F38-F37)/F37))*C37</f>
+        <v>1395.3316062176166</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>12203.839378238343</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>392137.76165803109</v>
+      </c>
+      <c r="F38">
+        <v>197</v>
+      </c>
+      <c r="G38">
+        <v>1723</v>
+      </c>
+      <c r="H38">
+        <v>55364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2022</v>
+      </c>
+      <c r="B39">
+        <v>2020</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ref="C39:C97" si="3">(1 + ((F39-F38)/F38))*C38</f>
+        <v>1416.5803108808288</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>12742.139896373055</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>400821.39896373055</v>
+      </c>
+      <c r="F39">
+        <v>200</v>
+      </c>
+      <c r="G39">
+        <v>1799</v>
+      </c>
+      <c r="H39">
+        <v>56590</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2023</v>
+      </c>
+      <c r="B40">
+        <v>2020</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>1444.9119170984454</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>13273.357512953367</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>409505.03626943001</v>
+      </c>
+      <c r="F40">
+        <v>204</v>
+      </c>
+      <c r="G40">
+        <v>1874</v>
+      </c>
+      <c r="H40">
+        <v>57816</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2024</v>
+      </c>
+      <c r="B41">
+        <v>2020</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>1473.243523316062</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>13811.658031088082</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>418181.59067357512</v>
+      </c>
+      <c r="F41">
+        <v>208</v>
+      </c>
+      <c r="G41">
+        <v>1950</v>
+      </c>
+      <c r="H41">
+        <v>59041</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42">
+        <v>2020</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="3"/>
+        <v>1501.5751295336786</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>14342.875647668392</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>426865.22797927458</v>
+      </c>
+      <c r="F42">
+        <v>212</v>
+      </c>
+      <c r="G42">
+        <v>2025</v>
+      </c>
+      <c r="H42">
+        <v>60267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2026</v>
+      </c>
+      <c r="B43">
+        <v>2020</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="3"/>
+        <v>1522.8238341968909</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>14881.176165803106</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>435541.78238341957</v>
+      </c>
+      <c r="F43">
+        <v>215</v>
+      </c>
+      <c r="G43">
+        <v>2101</v>
+      </c>
+      <c r="H43">
+        <v>61492</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2027</v>
+      </c>
+      <c r="B44">
+        <v>2020</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="3"/>
+        <v>1551.1554404145074</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>15412.393782383417</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>444225.41968911909</v>
+      </c>
+      <c r="F44">
+        <v>219</v>
+      </c>
+      <c r="G44">
+        <v>2176</v>
+      </c>
+      <c r="H44">
+        <v>62718</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2028</v>
+      </c>
+      <c r="B45">
+        <v>2020</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="3"/>
+        <v>1579.487046632124</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>15950.694300518131</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>452909.05699481856</v>
+      </c>
+      <c r="F45">
+        <v>223</v>
+      </c>
+      <c r="G45">
+        <v>2252</v>
+      </c>
+      <c r="H45">
+        <v>63944</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2029</v>
+      </c>
+      <c r="B46">
+        <v>2020</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="3"/>
+        <v>1600.7357512953365</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>16481.911917098441</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>461585.61139896361</v>
+      </c>
+      <c r="F46">
+        <v>226</v>
+      </c>
+      <c r="G46">
+        <v>2327</v>
+      </c>
+      <c r="H46">
+        <v>65169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2030</v>
+      </c>
+      <c r="B47">
+        <v>2020</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="3"/>
+        <v>1629.0673575129531</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>17020.212435233156</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>470269.24870466313</v>
+      </c>
+      <c r="F47">
+        <v>230</v>
+      </c>
+      <c r="G47">
+        <v>2403</v>
+      </c>
+      <c r="H47">
+        <v>66395</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2031</v>
+      </c>
+      <c r="B48">
+        <v>2020</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="3"/>
+        <v>1657.3989637305694</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>17636.424870466315</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>479122.87564766826</v>
+      </c>
+      <c r="F48">
+        <v>234</v>
+      </c>
+      <c r="G48">
+        <v>2490</v>
+      </c>
+      <c r="H48">
+        <v>67645</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2032</v>
+      </c>
+      <c r="B49">
+        <v>2020</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="3"/>
+        <v>1678.6476683937817</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>18259.720207253878</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>487976.50259067334</v>
+      </c>
+      <c r="F49">
+        <v>237</v>
+      </c>
+      <c r="G49">
+        <v>2578</v>
+      </c>
+      <c r="H49">
+        <v>68895</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2033</v>
+      </c>
+      <c r="B50">
+        <v>2020</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="3"/>
+        <v>1706.9792746113983</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>18883.015544041446</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>496830.12953367858</v>
+      </c>
+      <c r="F50">
+        <v>241</v>
+      </c>
+      <c r="G50">
+        <v>2666</v>
+      </c>
+      <c r="H50">
+        <v>70145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2034</v>
+      </c>
+      <c r="B51">
+        <v>2020</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="3"/>
+        <v>1735.3108808290149</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>19506.310880829009</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>505676.67357512936</v>
+      </c>
+      <c r="F51">
+        <v>245</v>
+      </c>
+      <c r="G51">
+        <v>2754</v>
+      </c>
+      <c r="H51">
+        <v>71394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2035</v>
+      </c>
+      <c r="B52">
+        <v>2020</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>1756.5595854922271</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>20129.606217616572</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>514530.30051813449</v>
+      </c>
+      <c r="F52">
+        <v>248</v>
+      </c>
+      <c r="G52">
+        <v>2842</v>
+      </c>
+      <c r="H52">
+        <v>72644</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2036</v>
+      </c>
+      <c r="B53">
+        <v>2020</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="3"/>
+        <v>1784.8911917098437</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>20745.818652849732</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>523383.92746113968</v>
+      </c>
+      <c r="F53">
+        <v>252</v>
+      </c>
+      <c r="G53">
+        <v>2929</v>
+      </c>
+      <c r="H53">
+        <v>73894</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2037</v>
+      </c>
+      <c r="B54">
+        <v>2020</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="3"/>
+        <v>1813.2227979274601</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>21369.113989637292</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>532237.55440414476</v>
+      </c>
+      <c r="F54">
+        <v>256</v>
+      </c>
+      <c r="G54">
+        <v>3017</v>
+      </c>
+      <c r="H54">
+        <v>75144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2038</v>
+      </c>
+      <c r="B55">
+        <v>2020</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="3"/>
+        <v>1834.4715025906726</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>21992.409326424859</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>541091.18134714989</v>
+      </c>
+      <c r="F55">
+        <v>259</v>
+      </c>
+      <c r="G55">
+        <v>3105</v>
+      </c>
+      <c r="H55">
+        <v>76394</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2039</v>
+      </c>
+      <c r="B56">
+        <v>2020</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="3"/>
+        <v>1862.8031088082892</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>22615.704663212422</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>549944.80829015514</v>
+      </c>
+      <c r="F56">
+        <v>263</v>
+      </c>
+      <c r="G56">
+        <v>3193</v>
+      </c>
+      <c r="H56">
+        <v>77644</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2040</v>
+      </c>
+      <c r="B57">
+        <v>2020</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="3"/>
+        <v>1891.1347150259055</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>23231.917098445578</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>558798.43523316027</v>
+      </c>
+      <c r="F57">
+        <v>267</v>
+      </c>
+      <c r="G57">
+        <v>3280</v>
+      </c>
+      <c r="H57">
+        <v>78894</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2041</v>
+      </c>
+      <c r="B58">
+        <v>2020</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="3"/>
+        <v>1919.4663212435221</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>23904.792746113977</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>568785.32642487017</v>
+      </c>
+      <c r="F58">
+        <v>271</v>
+      </c>
+      <c r="G58">
+        <v>3375</v>
+      </c>
+      <c r="H58">
+        <v>80304</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2042</v>
+      </c>
+      <c r="B59">
+        <v>2020</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="3"/>
+        <v>1947.7979274611387</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>24584.751295336773</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>578772.21761657996</v>
+      </c>
+      <c r="F59">
+        <v>275</v>
+      </c>
+      <c r="G59">
+        <v>3471</v>
+      </c>
+      <c r="H59">
+        <v>81714</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2043</v>
+      </c>
+      <c r="B60">
+        <v>2020</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="3"/>
+        <v>1976.1295336787555</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>25257.626943005169</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>588759.10880828986</v>
+      </c>
+      <c r="F60">
+        <v>279</v>
+      </c>
+      <c r="G60">
+        <v>3566</v>
+      </c>
+      <c r="H60">
+        <v>83124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2044</v>
+      </c>
+      <c r="B61">
+        <v>2020</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="3"/>
+        <v>2004.4611398963718</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>25930.502590673561</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>598753.08290155407</v>
+      </c>
+      <c r="F61">
+        <v>283</v>
+      </c>
+      <c r="G61">
+        <v>3661</v>
+      </c>
+      <c r="H61">
+        <v>84535</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2045</v>
+      </c>
+      <c r="B62">
+        <v>2020</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="3"/>
+        <v>2032.7927461139886</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>26603.378238341957</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>608739.97409326397</v>
+      </c>
+      <c r="F62">
+        <v>287</v>
+      </c>
+      <c r="G62">
+        <v>3756</v>
+      </c>
+      <c r="H62">
+        <v>85945</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2046</v>
+      </c>
+      <c r="B63">
+        <v>2020</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="3"/>
+        <v>2061.1243523316052</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>27276.253886010349</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>618726.86528497376</v>
+      </c>
+      <c r="F63">
+        <v>291</v>
+      </c>
+      <c r="G63">
+        <v>3851</v>
+      </c>
+      <c r="H63">
+        <v>87355</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2047</v>
+      </c>
+      <c r="B64">
+        <v>2020</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="3"/>
+        <v>2096.5388601036257</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>27949.129533678741</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>628713.75647668354</v>
+      </c>
+      <c r="F64">
+        <v>296</v>
+      </c>
+      <c r="G64">
+        <v>3946</v>
+      </c>
+      <c r="H64">
+        <v>88765</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2048</v>
+      </c>
+      <c r="B65">
+        <v>2020</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="3"/>
+        <v>2124.8704663212425</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>28622.005181347136</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>638707.73056994786</v>
+      </c>
+      <c r="F65">
+        <v>300</v>
+      </c>
+      <c r="G65">
+        <v>4041</v>
+      </c>
+      <c r="H65">
+        <v>90176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2049</v>
+      </c>
+      <c r="B66">
+        <v>2020</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="3"/>
+        <v>2153.2020725388593</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>29294.880829015536</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>648694.62176165776</v>
+      </c>
+      <c r="F66">
+        <v>304</v>
+      </c>
+      <c r="G66">
+        <v>4136</v>
+      </c>
+      <c r="H66">
+        <v>91586</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>2050</v>
+      </c>
+      <c r="B67">
+        <v>2020</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="3"/>
+        <v>2181.5336787564756</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D97" si="4">G67 * (C67/F67)</f>
+        <v>29967.756476683924</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E97" si="5">H67*(C67/F67)</f>
+        <v>658681.51295336755</v>
+      </c>
+      <c r="F67">
+        <v>308</v>
+      </c>
+      <c r="G67">
+        <v>4231</v>
+      </c>
+      <c r="H67">
+        <v>92996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>2051</v>
+      </c>
+      <c r="B68">
+        <v>2020</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="3"/>
+        <v>2209.865284974092</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="4"/>
+        <v>30598.134715025888</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="5"/>
+        <v>668052.19170984416</v>
+      </c>
+      <c r="F68">
+        <v>312</v>
+      </c>
+      <c r="G68">
+        <v>4320</v>
+      </c>
+      <c r="H68">
+        <v>94319</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>2052</v>
+      </c>
+      <c r="B69">
+        <v>2020</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="3"/>
+        <v>2231.1139896373043</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="4"/>
+        <v>31228.512953367859</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="5"/>
+        <v>677422.87046632089</v>
+      </c>
+      <c r="F69">
+        <v>315</v>
+      </c>
+      <c r="G69">
+        <v>4409</v>
+      </c>
+      <c r="H69">
+        <v>95642</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2053</v>
+      </c>
+      <c r="B70">
+        <v>2020</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="3"/>
+        <v>2259.4455958549206</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="4"/>
+        <v>31851.808290155419</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="5"/>
+        <v>686793.54922279739</v>
+      </c>
+      <c r="F70">
+        <v>319</v>
+      </c>
+      <c r="G70">
+        <v>4497</v>
+      </c>
+      <c r="H70">
+        <v>96965</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2054</v>
+      </c>
+      <c r="B71">
+        <v>2020</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="3"/>
+        <v>2287.7772020725374</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="4"/>
+        <v>32482.18652849739</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="5"/>
+        <v>696164.22797927423</v>
+      </c>
+      <c r="F71">
+        <v>323</v>
+      </c>
+      <c r="G71">
+        <v>4586</v>
+      </c>
+      <c r="H71">
+        <v>98288</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>2055</v>
+      </c>
+      <c r="B72">
+        <v>2020</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="3"/>
+        <v>2309.0259067357501</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="4"/>
+        <v>33112.564766839365</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="5"/>
+        <v>705541.98963730538</v>
+      </c>
+      <c r="F72">
+        <v>326</v>
+      </c>
+      <c r="G72">
+        <v>4675</v>
+      </c>
+      <c r="H72">
+        <v>99612</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>2056</v>
+      </c>
+      <c r="B73">
+        <v>2020</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="3"/>
+        <v>2337.3575129533665</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="4"/>
+        <v>33735.860103626925</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="5"/>
+        <v>714912.66839378199</v>
+      </c>
+      <c r="F73">
+        <v>330</v>
+      </c>
+      <c r="G73">
+        <v>4763</v>
+      </c>
+      <c r="H73">
+        <v>100935</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2057</v>
+      </c>
+      <c r="B74">
+        <v>2020</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="3"/>
+        <v>2365.6891191709833</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="4"/>
+        <v>34366.238341968899</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="5"/>
+        <v>724283.34715025872</v>
+      </c>
+      <c r="F74">
+        <v>334</v>
+      </c>
+      <c r="G74">
+        <v>4852</v>
+      </c>
+      <c r="H74">
+        <v>102258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2058</v>
+      </c>
+      <c r="B75">
+        <v>2020</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="3"/>
+        <v>2394.0207253886001</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="4"/>
+        <v>34996.616580310867</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="5"/>
+        <v>733654.02590673545</v>
+      </c>
+      <c r="F75">
+        <v>338</v>
+      </c>
+      <c r="G75">
+        <v>4941</v>
+      </c>
+      <c r="H75">
+        <v>103581</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>2059</v>
+      </c>
+      <c r="B76">
+        <v>2020</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="3"/>
+        <v>2415.2694300518124</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="4"/>
+        <v>35619.911917098427</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="5"/>
+        <v>743024.70466321206</v>
+      </c>
+      <c r="F76">
+        <v>341</v>
+      </c>
+      <c r="G76">
+        <v>5029</v>
+      </c>
+      <c r="H76">
+        <v>104904</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2060</v>
+      </c>
+      <c r="B77">
+        <v>2020</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="3"/>
+        <v>2443.6010362694287</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="4"/>
+        <v>36250.290155440394</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="5"/>
+        <v>752395.38341968867</v>
+      </c>
+      <c r="F77">
+        <v>345</v>
+      </c>
+      <c r="G77">
+        <v>5118</v>
+      </c>
+      <c r="H77">
+        <v>106227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2061</v>
+      </c>
+      <c r="B78">
+        <v>2020</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="3"/>
+        <v>2464.849740932641</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="4"/>
+        <v>36824.005181347129</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="5"/>
+        <v>760597.38341968867</v>
+      </c>
+      <c r="F78">
+        <v>348</v>
+      </c>
+      <c r="G78">
+        <v>5199</v>
+      </c>
+      <c r="H78">
+        <v>107385</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2062</v>
+      </c>
+      <c r="B79">
+        <v>2020</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="3"/>
+        <v>2486.0984455958533</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="4"/>
+        <v>37397.720207253857</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="5"/>
+        <v>768792.30051813414</v>
+      </c>
+      <c r="F79">
+        <v>351</v>
+      </c>
+      <c r="G79">
+        <v>5280</v>
+      </c>
+      <c r="H79">
+        <v>108542</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2063</v>
+      </c>
+      <c r="B80">
+        <v>2020</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="3"/>
+        <v>2507.3471502590655</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="4"/>
+        <v>37971.435233160591</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="5"/>
+        <v>776994.30051813414</v>
+      </c>
+      <c r="F80">
+        <v>354</v>
+      </c>
+      <c r="G80">
+        <v>5361</v>
+      </c>
+      <c r="H80">
+        <v>109700</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2064</v>
+      </c>
+      <c r="B81">
+        <v>2020</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="3"/>
+        <v>2528.5958549222778</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="4"/>
+        <v>38545.150259067326</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="5"/>
+        <v>785189.21761657961</v>
+      </c>
+      <c r="F81">
+        <v>357</v>
+      </c>
+      <c r="G81">
+        <v>5442</v>
+      </c>
+      <c r="H81">
+        <v>110857</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2065</v>
+      </c>
+      <c r="B82">
+        <v>2020</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="3"/>
+        <v>2549.8445595854901</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="4"/>
+        <v>39118.865284974061</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="5"/>
+        <v>793391.21761657961</v>
+      </c>
+      <c r="F82">
+        <v>360</v>
+      </c>
+      <c r="G82">
+        <v>5523</v>
+      </c>
+      <c r="H82">
+        <v>112015</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2066</v>
+      </c>
+      <c r="B83">
+        <v>2020</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="3"/>
+        <v>2571.0932642487023</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="4"/>
+        <v>39692.580310880789</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="5"/>
+        <v>801586.13471502508</v>
+      </c>
+      <c r="F83">
+        <v>363</v>
+      </c>
+      <c r="G83">
+        <v>5604</v>
+      </c>
+      <c r="H83">
+        <v>113172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2067</v>
+      </c>
+      <c r="B84">
+        <v>2020</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="3"/>
+        <v>2592.3419689119146</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="4"/>
+        <v>40266.295336787523</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="5"/>
+        <v>809788.13471502508</v>
+      </c>
+      <c r="F84">
+        <v>366</v>
+      </c>
+      <c r="G84">
+        <v>5685</v>
+      </c>
+      <c r="H84">
+        <v>114330</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>2068</v>
+      </c>
+      <c r="B85">
+        <v>2020</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="3"/>
+        <v>2613.5906735751269</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="4"/>
+        <v>40832.927461139858</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="5"/>
+        <v>817983.05181347067</v>
+      </c>
+      <c r="F85">
+        <v>369</v>
+      </c>
+      <c r="G85">
+        <v>5765</v>
+      </c>
+      <c r="H85">
+        <v>115487</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2069</v>
+      </c>
+      <c r="B86">
+        <v>2020</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="3"/>
+        <v>2634.8393782383391</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="4"/>
+        <v>41406.642487046585</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="5"/>
+        <v>826185.05181347055</v>
+      </c>
+      <c r="F86">
+        <v>372</v>
+      </c>
+      <c r="G86">
+        <v>5846</v>
+      </c>
+      <c r="H86">
+        <v>116645</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2070</v>
+      </c>
+      <c r="B87">
+        <v>2020</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="3"/>
+        <v>2656.0880829015514</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="4"/>
+        <v>41980.35751295332</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="5"/>
+        <v>834379.96891191613</v>
+      </c>
+      <c r="F87">
+        <v>375</v>
+      </c>
+      <c r="G87">
+        <v>5927</v>
+      </c>
+      <c r="H87">
+        <v>117802</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>2071</v>
+      </c>
+      <c r="B88">
+        <v>2020</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="3"/>
+        <v>2677.3367875647637</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="4"/>
+        <v>42589.487046632072</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="5"/>
+        <v>843056.52331606112</v>
+      </c>
+      <c r="F88">
+        <v>378</v>
+      </c>
+      <c r="G88">
+        <v>6013</v>
+      </c>
+      <c r="H88">
+        <v>119027</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2072</v>
+      </c>
+      <c r="B89">
+        <v>2020</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="3"/>
+        <v>2705.6683937823805</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="4"/>
+        <v>43198.616580310831</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="5"/>
+        <v>851733.07772020635</v>
+      </c>
+      <c r="F89">
+        <v>382</v>
+      </c>
+      <c r="G89">
+        <v>6099</v>
+      </c>
+      <c r="H89">
+        <v>120252</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2073</v>
+      </c>
+      <c r="B90">
+        <v>2020</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="3"/>
+        <v>2726.9170984455932</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="4"/>
+        <v>43800.663212435189</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="5"/>
+        <v>860409.63212435145</v>
+      </c>
+      <c r="F90">
+        <v>385</v>
+      </c>
+      <c r="G90">
+        <v>6184</v>
+      </c>
+      <c r="H90">
+        <v>121477</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>2074</v>
+      </c>
+      <c r="B91">
+        <v>2020</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="3"/>
+        <v>2748.1658031088054</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="4"/>
+        <v>44409.792746113941</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="5"/>
+        <v>869086.18652849644</v>
+      </c>
+      <c r="F91">
+        <v>388</v>
+      </c>
+      <c r="G91">
+        <v>6270</v>
+      </c>
+      <c r="H91">
+        <v>122702</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2075</v>
+      </c>
+      <c r="B92">
+        <v>2020</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="3"/>
+        <v>2769.4145077720177</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="4"/>
+        <v>45011.839378238292</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="5"/>
+        <v>877755.65803108714</v>
+      </c>
+      <c r="F92">
+        <v>391</v>
+      </c>
+      <c r="G92">
+        <v>6355</v>
+      </c>
+      <c r="H92">
+        <v>123926</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>2076</v>
+      </c>
+      <c r="B93">
+        <v>2020</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="3"/>
+        <v>2790.66321243523</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="4"/>
+        <v>45620.968911917051</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="5"/>
+        <v>886432.21243523224</v>
+      </c>
+      <c r="F93">
+        <v>394</v>
+      </c>
+      <c r="G93">
+        <v>6441</v>
+      </c>
+      <c r="H93">
+        <v>125151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>2077</v>
+      </c>
+      <c r="B94">
+        <v>2020</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="3"/>
+        <v>2818.9948186528468</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="4"/>
+        <v>46230.098445595802</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="5"/>
+        <v>895108.76683937723</v>
+      </c>
+      <c r="F94">
+        <v>398</v>
+      </c>
+      <c r="G94">
+        <v>6527</v>
+      </c>
+      <c r="H94">
+        <v>126376</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>2078</v>
+      </c>
+      <c r="B95">
+        <v>2020</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="3"/>
+        <v>2840.2435233160595</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="4"/>
+        <v>46832.145077720161</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="5"/>
+        <v>903785.32124352246</v>
+      </c>
+      <c r="F95">
+        <v>401</v>
+      </c>
+      <c r="G95">
+        <v>6612</v>
+      </c>
+      <c r="H95">
+        <v>127601</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>2079</v>
+      </c>
+      <c r="B96">
+        <v>2020</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="3"/>
+        <v>2861.4922279792722</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="4"/>
+        <v>47441.274611398927</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="5"/>
+        <v>912461.87564766768</v>
+      </c>
+      <c r="F96">
+        <v>404</v>
+      </c>
+      <c r="G96">
+        <v>6698</v>
+      </c>
+      <c r="H96">
+        <v>128826</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2080</v>
+      </c>
+      <c r="B97">
+        <v>2020</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="3"/>
+        <v>2882.7409326424845</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="4"/>
+        <v>48043.321243523278</v>
+      </c>
+      <c r="E97">
+        <f>H97*(C97/F97)</f>
+        <v>921131.34715025825</v>
+      </c>
+      <c r="F97">
+        <v>407</v>
+      </c>
+      <c r="G97">
+        <v>6783</v>
+      </c>
+      <c r="H97">
+        <v>130050</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDED922-4E4D-49CD-91EB-13A869C9251E}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -9145,7 +11991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3BFB63-2E02-4377-818A-45B8B0FF335A}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>

</xml_diff>